<commit_message>
Add forest growth curve to natural regeneration forest.
</commit_message>
<xml_diff>
--- a/individual/ForestCsink/Table4_7-10.xlsx
+++ b/individual/ForestCsink/Table4_7-10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\LandUse_ForestCSink\AIMPLUM\individual\ForestCsink\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\LandUse_master\AIMPLUM\individual\ForestCsink\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF8EF625-B591-4A90-B403-F13BBE4873DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3B4043-ABFF-4F28-B2A2-4556D63E9653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2208" yWindow="4320" windowWidth="17280" windowHeight="9108" activeTab="2"/>
+    <workbookView minimized="1" xWindow="1716" yWindow="876" windowWidth="12324" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -221,9 +221,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -284,24 +284,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -608,24 +605,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:D39"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="24.5" customWidth="1"/>
+    <col min="3" max="4" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
@@ -633,7 +630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
@@ -641,7 +638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -649,7 +646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -657,7 +654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
@@ -665,7 +662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
@@ -673,7 +670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
@@ -681,7 +678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
@@ -689,7 +686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
@@ -697,7 +694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
@@ -705,7 +702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
@@ -713,7 +710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
@@ -721,7 +718,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
@@ -729,7 +726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
@@ -737,7 +734,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
@@ -745,7 +742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>23</v>
       </c>
@@ -753,7 +750,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
         <v>25</v>
       </c>
@@ -761,7 +758,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
         <v>25</v>
       </c>
@@ -769,7 +766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
         <v>27</v>
       </c>
@@ -777,7 +774,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
@@ -785,7 +782,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
@@ -793,7 +790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
         <v>29</v>
       </c>
@@ -801,7 +798,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>31</v>
       </c>
@@ -809,7 +806,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>31</v>
       </c>
@@ -817,7 +814,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>33</v>
       </c>
@@ -825,7 +822,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>33</v>
       </c>
@@ -833,7 +830,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
         <v>35</v>
       </c>
@@ -841,7 +838,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
         <v>35</v>
       </c>
@@ -849,7 +846,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
         <v>37</v>
       </c>
@@ -857,7 +854,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
         <v>37</v>
       </c>
@@ -865,7 +862,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>39</v>
       </c>
@@ -873,7 +870,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
         <v>39</v>
       </c>
@@ -881,7 +878,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
         <v>41</v>
       </c>
@@ -889,7 +886,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
         <v>41</v>
       </c>
@@ -897,7 +894,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>43</v>
       </c>
@@ -905,7 +902,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
         <v>43</v>
       </c>
@@ -913,7 +910,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
         <v>45</v>
       </c>
@@ -921,7 +918,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
         <v>45</v>
       </c>
@@ -937,19 +934,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
       <selection sqref="A1:IV1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -969,8 +966,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -982,7 +979,7 @@
       <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <f>(280+350)/2</f>
         <v>315</v>
       </c>
@@ -994,8 +991,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1007,7 +1004,7 @@
       <c r="D3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <f>(280+350)/2</f>
         <v>315</v>
       </c>
@@ -1019,8 +1016,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1032,7 +1029,7 @@
       <c r="D4" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <f>(180+290)/2</f>
         <v>235</v>
       </c>
@@ -1044,8 +1041,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1057,7 +1054,7 @@
       <c r="D5" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <f>(180+290)/2</f>
         <v>235</v>
       </c>
@@ -1069,8 +1066,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1094,8 +1091,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1119,8 +1116,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1144,8 +1141,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1169,8 +1166,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1194,8 +1191,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1219,8 +1216,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1244,8 +1241,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1269,8 +1266,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1294,8 +1291,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1319,8 +1316,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1344,8 +1341,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1369,8 +1366,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1386,8 +1383,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1403,8 +1400,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1428,8 +1425,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1453,8 +1450,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1477,8 +1474,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1501,8 +1498,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1525,8 +1522,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1549,8 +1546,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1566,8 +1563,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1583,8 +1580,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1600,8 +1597,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1617,8 +1614,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1641,8 +1638,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1665,8 +1662,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1689,8 +1686,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1713,8 +1710,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1737,8 +1734,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1761,8 +1758,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1785,8 +1782,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1809,8 +1806,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1826,8 +1823,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1843,8 +1840,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1867,8 +1864,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A41" s="2" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1891,8 +1888,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="2" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1915,8 +1912,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A43" s="2" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1939,8 +1936,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1963,8 +1960,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A45" s="2" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1987,8 +1984,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A46" s="2" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2010,8 +2007,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A47" s="2" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>4</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2033,8 +2030,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A48" s="2" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>4</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2058,8 +2055,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A49" s="2" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2083,8 +2080,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A50" s="2" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>6</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2100,8 +2097,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A51" s="2" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>6</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2117,8 +2114,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A52" s="2" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2141,8 +2138,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A53" s="2" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>6</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2165,8 +2162,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A54" s="2" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>6</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2188,8 +2185,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2211,8 +2208,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A56" s="2" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>6</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2228,8 +2225,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A57" s="2" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2245,8 +2242,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A58" s="2" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>6</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2269,8 +2266,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A59" s="2" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>6</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2293,8 +2290,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A60" s="2" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2317,8 +2314,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A61" s="2" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2341,8 +2338,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A62" s="2" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2365,8 +2362,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A63" s="2" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2389,8 +2386,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A64" s="2" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -2406,8 +2403,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>7</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2423,8 +2420,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A66" s="2" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>7</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2440,8 +2437,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A67" s="2" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -2457,8 +2454,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A68" s="2" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -2481,8 +2478,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A69" s="2" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2505,8 +2502,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A70" s="2" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>8</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2529,8 +2526,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A71" s="2" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>8</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -2553,8 +2550,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A72" s="2" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>8</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -2577,8 +2574,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A73" s="2" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>8</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -2601,8 +2598,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A74" s="2" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>8</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2625,8 +2622,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A75" s="2" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>8</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -2649,8 +2646,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -2666,8 +2663,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A77" s="3" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -2683,8 +2680,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A78" s="2" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>4</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -2707,8 +2704,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A79" s="2" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>4</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -2731,8 +2728,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A80" s="2" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>4</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -2755,8 +2752,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A81" s="2" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>4</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -2779,8 +2776,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A82" s="2" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>4</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -2803,8 +2800,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A83" s="2" t="s">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>4</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -2827,8 +2824,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A84" s="2" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>4</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -2851,8 +2848,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A85" s="2" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>4</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -2875,8 +2872,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A86" s="2" t="s">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>4</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -2900,8 +2897,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A87" s="2" t="s">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>4</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -2925,8 +2922,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A88" s="2" t="s">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>6</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -2949,8 +2946,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A89" s="2" t="s">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>6</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -2973,8 +2970,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A90" s="2" t="s">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>6</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -2997,8 +2994,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A91" s="2" t="s">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>6</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -3021,8 +3018,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A92" s="2" t="s">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>6</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -3045,8 +3042,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A93" s="2" t="s">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>6</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -3069,8 +3066,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A94" s="2" t="s">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>6</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -3086,8 +3083,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A95" s="2" t="s">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>6</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -3103,8 +3100,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A96" s="2" t="s">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>6</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -3128,8 +3125,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A97" s="2" t="s">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>6</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -3153,8 +3150,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A98" s="2" t="s">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -3178,8 +3175,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A99" s="2" t="s">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>7</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -3203,8 +3200,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A100" s="2" t="s">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>7</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -3227,8 +3224,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A101" s="2" t="s">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>7</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -3251,8 +3248,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A102" s="2" t="s">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="1" t="s">
@@ -3268,8 +3265,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A103" s="2" t="s">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>7</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -3285,8 +3282,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A104" s="2" t="s">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>7</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -3302,8 +3299,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A105" s="2" t="s">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>7</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -3319,8 +3316,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A106" s="2" t="s">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>7</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -3343,8 +3340,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A107" s="2" t="s">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>7</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -3367,8 +3364,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A108" s="2" t="s">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>8</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -3391,8 +3388,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A109" s="2" t="s">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>8</v>
       </c>
       <c r="B109" s="1" t="s">
@@ -3415,8 +3412,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A110" s="2" t="s">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -3439,8 +3436,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A111" s="2" t="s">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>8</v>
       </c>
       <c r="B111" s="1" t="s">
@@ -3463,8 +3460,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A112" s="2" t="s">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>8</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -3487,8 +3484,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A113" s="2" t="s">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>8</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -3511,8 +3508,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A114" s="3" t="s">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -3528,8 +3525,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A115" s="3" t="s">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -3546,28 +3543,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G115"/>
+  <autoFilter ref="A1:G115" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="10.25" customWidth="1"/>
-    <col min="7" max="7" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3587,8 +3584,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3610,8 +3607,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3633,8 +3630,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -3656,8 +3653,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3679,8 +3676,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -3703,8 +3700,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -3727,8 +3724,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -3750,8 +3747,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3773,8 +3770,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -3798,8 +3795,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -3823,8 +3820,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -3846,8 +3843,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3869,8 +3866,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -3893,8 +3890,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -3917,8 +3914,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -3940,8 +3937,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3963,8 +3960,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -3980,8 +3977,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -3997,8 +3994,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -4022,8 +4019,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -4047,8 +4044,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -4064,8 +4061,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -4081,8 +4078,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -4104,8 +4101,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -4127,8 +4124,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -4144,8 +4141,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -4161,8 +4158,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -4178,8 +4175,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -4195,8 +4192,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -4218,8 +4215,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -4241,8 +4238,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -4266,8 +4263,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -4291,8 +4288,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -4314,8 +4311,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -4337,8 +4334,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -4362,8 +4359,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -4387,8 +4384,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -4404,8 +4401,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -4421,8 +4418,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -4445,8 +4442,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A41" s="2" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -4469,8 +4466,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="2" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -4493,8 +4490,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A43" s="2" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -4517,8 +4514,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -4533,7 +4530,7 @@
       <c r="E44">
         <v>2.4</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="4">
         <f>(13+8+10)/3</f>
         <v>10.333333333333334</v>
       </c>
@@ -4541,8 +4538,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A45" s="2" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -4557,15 +4554,15 @@
       <c r="E45">
         <v>1.8</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="4">
         <v>10</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A46" s="2" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -4581,7 +4578,7 @@
         <f>(0.2+0.7)/2</f>
         <v>0.44999999999999996</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F46" s="4">
         <f>(5+3+15)/3</f>
         <v>7.666666666666667</v>
       </c>
@@ -4589,8 +4586,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A47" s="2" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>4</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -4605,7 +4602,7 @@
       <c r="E47">
         <v>0.9</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="4">
         <f>(8+2.5+10)/3</f>
         <v>6.833333333333333</v>
       </c>
@@ -4613,8 +4610,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A48" s="2" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>4</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -4637,8 +4634,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A49" s="2" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -4661,8 +4658,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A50" s="2" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>6</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -4678,8 +4675,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A51" s="2" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>6</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -4695,8 +4692,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A52" s="2" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -4711,7 +4708,7 @@
       <c r="E52">
         <v>2.4</v>
       </c>
-      <c r="F52" s="5">
+      <c r="F52" s="4">
         <f>(13+8+10)/3</f>
         <v>10.333333333333334</v>
       </c>
@@ -4719,8 +4716,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A53" s="2" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>6</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -4742,8 +4739,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A54" s="2" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>6</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -4758,7 +4755,7 @@
       <c r="E54">
         <v>1.2</v>
       </c>
-      <c r="F54" s="5">
+      <c r="F54" s="4">
         <f>(5+3+15)/3</f>
         <v>7.666666666666667</v>
       </c>
@@ -4766,8 +4763,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -4782,7 +4779,7 @@
       <c r="E55">
         <v>0.9</v>
       </c>
-      <c r="F55" s="5">
+      <c r="F55" s="4">
         <f>(8+2.5+10)/3</f>
         <v>6.833333333333333</v>
       </c>
@@ -4790,8 +4787,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A56" s="2" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>6</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -4807,8 +4804,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A57" s="2" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -4824,8 +4821,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A58" s="2" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>6</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -4848,8 +4845,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A59" s="2" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>6</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -4872,8 +4869,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A60" s="2" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -4895,8 +4892,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A61" s="2" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -4918,8 +4915,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A62" s="2" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -4941,8 +4938,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A63" s="2" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -4964,8 +4961,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A64" s="2" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -4981,8 +4978,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>7</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -4998,8 +4995,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A66" s="2" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>7</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -5015,8 +5012,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A67" s="2" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -5032,8 +5029,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A68" s="2" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -5055,8 +5052,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A69" s="2" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -5078,8 +5075,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A70" s="2" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>8</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -5103,8 +5100,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A71" s="2" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>8</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -5128,8 +5125,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A72" s="2" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>8</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -5151,8 +5148,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A73" s="2" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>8</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -5174,8 +5171,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A74" s="2" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>8</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -5199,8 +5196,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A75" s="2" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>8</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -5224,8 +5221,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -5241,8 +5238,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A77" s="3" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -5258,8 +5255,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A78" s="2" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>4</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -5271,10 +5268,10 @@
       <c r="D78" t="s">
         <v>49</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E78" s="5">
         <v>11</v>
       </c>
-      <c r="F78" s="5">
+      <c r="F78" s="4">
         <f>(20+20+15+20)/4</f>
         <v>18.75</v>
       </c>
@@ -5282,8 +5279,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A79" s="2" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>4</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -5295,10 +5292,10 @@
       <c r="D79" t="s">
         <v>48</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E79" s="5">
         <v>3.1</v>
       </c>
-      <c r="F79" s="5">
+      <c r="F79" s="4">
         <f>(20+20+15+20)/4</f>
         <v>18.75</v>
       </c>
@@ -5306,8 +5303,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A80" s="2" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>4</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -5322,7 +5319,7 @@
       <c r="E80">
         <v>7</v>
       </c>
-      <c r="F80" s="5">
+      <c r="F80" s="4">
         <f>(16+7+8+(6+20)/2)/4</f>
         <v>11</v>
       </c>
@@ -5330,8 +5327,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A81" s="2" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>4</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -5346,7 +5343,7 @@
       <c r="E81">
         <v>2</v>
       </c>
-      <c r="F81" s="5">
+      <c r="F81" s="4">
         <f>(16+7+8+(6+20)/2)/4</f>
         <v>11</v>
       </c>
@@ -5354,8 +5351,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A82" s="2" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>4</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -5370,7 +5367,7 @@
       <c r="E82">
         <v>4</v>
       </c>
-      <c r="F82" s="5">
+      <c r="F82" s="4">
         <f>(20+7+8+10)/4</f>
         <v>11.25</v>
       </c>
@@ -5378,8 +5375,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A83" s="2" t="s">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>4</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -5394,7 +5391,7 @@
       <c r="E83">
         <v>1</v>
       </c>
-      <c r="F83" s="5">
+      <c r="F83" s="4">
         <f>(20+7+8+10)/4</f>
         <v>11.25</v>
       </c>
@@ -5402,8 +5399,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A84" s="2" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>4</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -5418,7 +5415,7 @@
       <c r="E84">
         <v>4</v>
       </c>
-      <c r="F84" s="5">
+      <c r="F84" s="4">
         <f>(20+5)/2</f>
         <v>12.5</v>
       </c>
@@ -5426,8 +5423,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A85" s="2" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>4</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -5442,7 +5439,7 @@
       <c r="E85">
         <v>1</v>
       </c>
-      <c r="F85" s="5">
+      <c r="F85" s="4">
         <f>(20+5)/2</f>
         <v>12.5</v>
       </c>
@@ -5450,8 +5447,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A86" s="2" t="s">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>4</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -5467,7 +5464,7 @@
         <f>(1.8+5)/2</f>
         <v>3.4</v>
       </c>
-      <c r="F86" s="5">
+      <c r="F86" s="4">
         <f>(10+10+2+4)/4</f>
         <v>6.5</v>
       </c>
@@ -5475,8 +5472,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A87" s="2" t="s">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>4</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -5492,7 +5489,7 @@
         <f>(0.4+1.4)/2</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="F87" s="5">
+      <c r="F87" s="4">
         <f>(10+10+2+4)/4</f>
         <v>6.5</v>
       </c>
@@ -5500,8 +5497,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A88" s="2" t="s">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>6</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -5516,7 +5513,7 @@
       <c r="E88">
         <v>7</v>
       </c>
-      <c r="F88" s="5">
+      <c r="F88" s="4">
         <f>(20+7+8+10)/4</f>
         <v>11.25</v>
       </c>
@@ -5524,8 +5521,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A89" s="2" t="s">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>6</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -5540,7 +5537,7 @@
       <c r="E89">
         <v>2</v>
       </c>
-      <c r="F89" s="5">
+      <c r="F89" s="4">
         <f>(20+7+8+10)/4</f>
         <v>11.25</v>
       </c>
@@ -5548,8 +5545,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A90" s="2" t="s">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>6</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -5564,7 +5561,7 @@
       <c r="E90">
         <v>4</v>
       </c>
-      <c r="F90" s="5">
+      <c r="F90" s="4">
         <f>(20+7+8+10)/4</f>
         <v>11.25</v>
       </c>
@@ -5572,8 +5569,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A91" s="2" t="s">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>6</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -5588,7 +5585,7 @@
       <c r="E91">
         <v>1</v>
       </c>
-      <c r="F91" s="5">
+      <c r="F91" s="4">
         <f>(20+7+8+10)/4</f>
         <v>11.25</v>
       </c>
@@ -5596,8 +5593,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A92" s="2" t="s">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>6</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -5612,7 +5609,7 @@
       <c r="E92">
         <v>4</v>
       </c>
-      <c r="F92" s="5">
+      <c r="F92" s="4">
         <f>(20+5)/2</f>
         <v>12.5</v>
       </c>
@@ -5620,8 +5617,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A93" s="2" t="s">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>6</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -5636,7 +5633,7 @@
       <c r="E93">
         <v>1</v>
       </c>
-      <c r="F93" s="5">
+      <c r="F93" s="4">
         <f>(20+5)/2</f>
         <v>12.5</v>
       </c>
@@ -5644,8 +5641,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A94" s="2" t="s">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>6</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -5661,8 +5658,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A95" s="2" t="s">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>6</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -5678,8 +5675,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A96" s="2" t="s">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>6</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -5703,8 +5700,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A97" s="2" t="s">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>6</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -5728,8 +5725,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A98" s="2" t="s">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -5753,8 +5750,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A99" s="2" t="s">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>7</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -5778,8 +5775,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A100" s="2" t="s">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>7</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -5801,8 +5798,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A101" s="2" t="s">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>7</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -5824,8 +5821,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A102" s="2" t="s">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="1" t="s">
@@ -5841,8 +5838,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A103" s="2" t="s">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>7</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -5858,8 +5855,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A104" s="2" t="s">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>7</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -5875,8 +5872,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A105" s="2" t="s">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>7</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -5892,8 +5889,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A106" s="2" t="s">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>7</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -5915,8 +5912,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A107" s="2" t="s">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>7</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -5938,8 +5935,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A108" s="2" t="s">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>8</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -5963,8 +5960,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A109" s="2" t="s">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>8</v>
       </c>
       <c r="B109" s="1" t="s">
@@ -5988,8 +5985,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A110" s="2" t="s">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -6011,8 +6008,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A111" s="2" t="s">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>8</v>
       </c>
       <c r="B111" s="1" t="s">
@@ -6034,8 +6031,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A112" s="2" t="s">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>8</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -6059,8 +6056,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A113" s="2" t="s">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>8</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -6084,8 +6081,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A114" s="3" t="s">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -6101,8 +6098,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A115" s="3" t="s">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -6119,7 +6116,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G115"/>
+  <autoFilter ref="A1:G115" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51200000000000001" footer="0.51200000000000001"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>